<commit_message>
fix: autoWidth default value
</commit_message>
<xml_diff>
--- a/tests/output/01-presets.xlsx
+++ b/tests/output/01-presets.xlsx
@@ -458,6 +458,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="9.2" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -501,6 +505,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="9.2" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -544,6 +552,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="9.2" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Remove conditionalStyle and fix autoWidth default value (#32)
* fix

* del: conditionalStyle

* fix

* fix: autoWidth default value
</commit_message>
<xml_diff>
--- a/tests/output/01-presets.xlsx
+++ b/tests/output/01-presets.xlsx
@@ -458,6 +458,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="9.2" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -501,6 +505,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="9.2" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -544,6 +552,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="9.2" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>